<commit_message>
finished up to mortality section
</commit_message>
<xml_diff>
--- a/write/tables/table_incidence.xlsx
+++ b/write/tables/table_incidence.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16660" windowHeight="17920" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-15140" windowWidth="21000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="incidence - formatted" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>All patients</t>
   </si>
@@ -68,20 +68,32 @@
     <t>Weekend</t>
   </si>
   <si>
-    <t>Baseline</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
     <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Baseline incidence</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>IRR (95%CI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,6 +117,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -122,8 +139,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -147,14 +184,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -166,6 +255,21 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -177,6 +281,21 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1364,677 +1483,1088 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q13"/>
+  <dimension ref="B2:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="10" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="3"/>
+    <col min="18" max="18" width="2.5" style="3" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="27" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B2" t="str">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B3" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B1</f>
         <v>idstr</v>
       </c>
-      <c r="D2" t="str">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!C1</f>
         <v>parm</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E3" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!D1</f>
         <v>label</v>
       </c>
-      <c r="F2" t="str">
-        <f>'tb_incidence_news_all - csv'!E1</f>
-        <v>estimate</v>
-      </c>
-      <c r="G2" t="str">
-        <f>'tb_incidence_news_all - csv'!F1</f>
-        <v>stderr</v>
-      </c>
-      <c r="H2" t="str">
-        <f>'tb_incidence_news_all - csv'!G1</f>
-        <v>z</v>
-      </c>
-      <c r="I2" t="str">
-        <f>'tb_incidence_news_all - csv'!H1</f>
-        <v>p</v>
-      </c>
-      <c r="J2" t="str">
-        <f>'tb_incidence_news_all - csv'!I1</f>
-        <v>stars</v>
-      </c>
-      <c r="K2" t="str">
-        <f>'tb_incidence_news_all - csv'!J1</f>
-        <v>min95</v>
-      </c>
-      <c r="L2" t="str">
-        <f>'tb_incidence_news_all - csv'!K1</f>
-        <v>max95</v>
-      </c>
-      <c r="M2" t="str">
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!L1</f>
         <v>table_order</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O3" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!M1</f>
         <v>model_sequence</v>
       </c>
-      <c r="O2">
+      <c r="P3" s="4">
         <f>'tb_incidence_news_all - csv'!N1</f>
         <v>0</v>
       </c>
+      <c r="Q3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!F1</f>
+        <v>stderr</v>
+      </c>
+      <c r="V3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!G1</f>
+        <v>z</v>
+      </c>
+      <c r="W3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!H1</f>
+        <v>p</v>
+      </c>
+      <c r="X3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!I1</f>
+        <v>stars</v>
+      </c>
+      <c r="Y3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!J1</f>
+        <v>min95</v>
+      </c>
+      <c r="Z3" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!K1</f>
+        <v>max95</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" t="str">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B4" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B2</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D4" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C2</f>
         <v>teaching_hosp</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E4" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D2</f>
         <v>(firstnm) teaching_hosp</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="1">
         <f>'tb_incidence_news_all - csv'!E2</f>
         <v>1.085</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="1">
         <f>'tb_incidence_news_all - csv'!F2</f>
         <v>3.7368150000000003E-2</v>
       </c>
-      <c r="H3">
+      <c r="H4" s="1">
         <f>'tb_incidence_news_all - csv'!G2</f>
         <v>2.3717831999999999</v>
       </c>
-      <c r="I3">
+      <c r="I4" s="1">
         <f>'tb_incidence_news_all - csv'!H2</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J4" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I2</f>
         <v>*</v>
       </c>
-      <c r="K3">
+      <c r="K4" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(L4,"0.000"),", ",TEXT(M4,"0.000"),")")</f>
+        <v>(1.014, 1.161)</v>
+      </c>
+      <c r="L4" s="8">
         <f>'tb_incidence_news_all - csv'!J2</f>
         <v>1.014</v>
       </c>
-      <c r="L3">
+      <c r="M4" s="8">
         <f>'tb_incidence_news_all - csv'!K2</f>
         <v>1.161</v>
       </c>
-      <c r="M3">
+      <c r="N4" s="1">
         <f>'tb_incidence_news_all - csv'!L2</f>
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="O4" s="1">
         <f>'tb_incidence_news_all - csv'!M2</f>
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="P4" s="1">
         <f>'tb_incidence_news_all - csv'!N2</f>
         <v>0</v>
       </c>
-      <c r="P3" s="1">
-        <f>I3</f>
+      <c r="Q4" s="3">
+        <f>I4</f>
         <v>1.7999999999999999E-2</v>
       </c>
+      <c r="S4" s="1">
+        <f>'tb_incidence_news_high - csv'!E2</f>
+        <v>1.113</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y4,"0.000"),", ",TEXT(Z4,"0.000"),")")</f>
+        <v>(1.027, 1.207)</v>
+      </c>
+      <c r="U4" s="1">
+        <f>'tb_incidence_news_high - csv'!F2</f>
+        <v>4.581557E-2</v>
+      </c>
+      <c r="V4" s="1">
+        <f>'tb_incidence_news_high - csv'!G2</f>
+        <v>2.6035943000000001</v>
+      </c>
+      <c r="W4" s="1">
+        <f>'tb_incidence_news_high - csv'!H2</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I2</f>
+        <v>**</v>
+      </c>
+      <c r="Y4" s="1">
+        <f>'tb_incidence_news_high - csv'!J2</f>
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="Z4" s="1">
+        <f>'tb_incidence_news_high - csv'!K2</f>
+        <v>1.2070000000000001</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>W4</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" t="str">
+    <row r="5" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B5" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B3</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D5" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C3</f>
         <v>hes_overnight_c</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E5" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D3</f>
         <v>(firstnm) hes_overnight_c</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="1">
         <f>'tb_incidence_news_all - csv'!E3</f>
         <v>1.0029999999999999</v>
       </c>
-      <c r="G4">
+      <c r="G5" s="1">
         <f>'tb_incidence_news_all - csv'!F3</f>
         <v>5.0294000000000001E-4</v>
       </c>
-      <c r="H4">
+      <c r="H5" s="1">
         <f>'tb_incidence_news_all - csv'!G3</f>
         <v>5.5298620999999999</v>
       </c>
-      <c r="I4">
+      <c r="I5" s="1">
         <f>'tb_incidence_news_all - csv'!H3</f>
         <v>0</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J5" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I3</f>
         <v>***</v>
       </c>
-      <c r="K4">
+      <c r="K5" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(L5,"0.000"),", ",TEXT(M5,"0.000"),")")</f>
+        <v>(1.002, 1.004)</v>
+      </c>
+      <c r="L5" s="8">
         <f>'tb_incidence_news_all - csv'!J3</f>
         <v>1.002</v>
       </c>
-      <c r="L4">
+      <c r="M5" s="8">
         <f>'tb_incidence_news_all - csv'!K3</f>
         <v>1.004</v>
       </c>
-      <c r="M4">
+      <c r="N5" s="1">
         <f>'tb_incidence_news_all - csv'!L3</f>
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="O5" s="1">
         <f>'tb_incidence_news_all - csv'!M3</f>
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="P5" s="1">
         <f>'tb_incidence_news_all - csv'!N3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>14</v>
+      <c r="Q5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="1">
+        <f>'tb_incidence_news_high - csv'!E3</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y5,"0.000"),", ",TEXT(Z5,"0.000"),")")</f>
+        <v>(1.004, 1.006)</v>
+      </c>
+      <c r="U5" s="1">
+        <f>'tb_incidence_news_high - csv'!F3</f>
+        <v>5.9048E-4</v>
+      </c>
+      <c r="V5" s="1">
+        <f>'tb_incidence_news_high - csv'!G3</f>
+        <v>9.0685230000000008</v>
+      </c>
+      <c r="W5" s="1">
+        <f>'tb_incidence_news_high - csv'!H3</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I3</f>
+        <v>***</v>
+      </c>
+      <c r="Y5" s="1">
+        <f>'tb_incidence_news_high - csv'!J3</f>
+        <v>1.004</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>'tb_incidence_news_high - csv'!K3</f>
+        <v>1.006</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="AA6" s="3"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" t="str">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B4</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D7" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C4</f>
         <v>0.ccot_shift_pattern</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E7" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D4</f>
         <v>(firstnm) ccot_shift_pattern</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="1">
         <f>'tb_incidence_news_all - csv'!E4</f>
         <v>0.55800000000000005</v>
       </c>
-      <c r="G6">
+      <c r="G7" s="1">
         <f>'tb_incidence_news_all - csv'!F4</f>
         <v>3.9176959999999997E-2</v>
       </c>
-      <c r="H6">
+      <c r="H7" s="1">
         <f>'tb_incidence_news_all - csv'!G4</f>
         <v>-8.3097942000000007</v>
       </c>
-      <c r="I6">
+      <c r="I7" s="1">
         <f>'tb_incidence_news_all - csv'!H4</f>
         <v>0</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J7" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I4</f>
         <v>***</v>
       </c>
-      <c r="K6">
+      <c r="K7" s="1" t="str">
+        <f t="shared" ref="K7:K9" si="0">CONCATENATE("(",TEXT(L7,"0.000"),", ",TEXT(M7,"0.000"),")")</f>
+        <v>(0.486, 0.640)</v>
+      </c>
+      <c r="L7" s="8">
         <f>'tb_incidence_news_all - csv'!J4</f>
         <v>0.48599999999999999</v>
       </c>
-      <c r="L6">
+      <c r="M7" s="8">
         <f>'tb_incidence_news_all - csv'!K4</f>
         <v>0.64</v>
       </c>
-      <c r="M6">
+      <c r="N7" s="1">
         <f>'tb_incidence_news_all - csv'!L4</f>
         <v>1</v>
       </c>
-      <c r="N6">
+      <c r="O7" s="1">
         <f>'tb_incidence_news_all - csv'!M4</f>
         <v>1</v>
       </c>
-      <c r="O6">
+      <c r="P7" s="1">
         <f>'tb_incidence_news_all - csv'!N4</f>
         <v>0</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>14</v>
+      <c r="Q7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="1">
+        <f>'tb_incidence_news_high - csv'!E4</f>
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y7,"0.000"),", ",TEXT(Z7,"0.000"),")")</f>
+        <v>(0.536, 0.743)</v>
+      </c>
+      <c r="U7" s="1">
+        <f>'tb_incidence_news_high - csv'!F4</f>
+        <v>5.2779260000000001E-2</v>
+      </c>
+      <c r="V7" s="1">
+        <f>'tb_incidence_news_high - csv'!G4</f>
+        <v>-5.5040937000000003</v>
+      </c>
+      <c r="W7" s="1">
+        <f>'tb_incidence_news_high - csv'!H4</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I4</f>
+        <v>***</v>
+      </c>
+      <c r="Y7" s="1">
+        <f>'tb_incidence_news_high - csv'!J4</f>
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="Z7" s="1">
+        <f>'tb_incidence_news_high - csv'!K4</f>
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" t="str">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B5</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D8" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C5</f>
         <v>1.ccot_shift_pattern</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E8" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D5</f>
         <v>(firstnm) ccot_shift_pattern</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="1">
         <f>'tb_incidence_news_all - csv'!E5</f>
         <v>0.57399999999999995</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="1">
         <f>'tb_incidence_news_all - csv'!F5</f>
         <v>2.0753509999999999E-2</v>
       </c>
-      <c r="H7">
+      <c r="H8" s="1">
         <f>'tb_incidence_news_all - csv'!G5</f>
         <v>-15.363903000000001</v>
       </c>
-      <c r="I7">
+      <c r="I8" s="1">
         <f>'tb_incidence_news_all - csv'!H5</f>
         <v>0</v>
       </c>
-      <c r="J7" t="str">
+      <c r="J8" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I5</f>
         <v>***</v>
       </c>
-      <c r="K7">
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(0.534, 0.616)</v>
+      </c>
+      <c r="L8" s="8">
         <f>'tb_incidence_news_all - csv'!J5</f>
         <v>0.53400000000000003</v>
       </c>
-      <c r="L7">
+      <c r="M8" s="8">
         <f>'tb_incidence_news_all - csv'!K5</f>
         <v>0.61599999999999999</v>
       </c>
-      <c r="M7">
+      <c r="N8" s="1">
         <f>'tb_incidence_news_all - csv'!L5</f>
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="O8" s="1">
         <f>'tb_incidence_news_all - csv'!M5</f>
         <v>1</v>
       </c>
-      <c r="O7">
+      <c r="P8" s="1">
         <f>'tb_incidence_news_all - csv'!N5</f>
         <v>0</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>14</v>
+      <c r="Q8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" s="1">
+        <f>'tb_incidence_news_high - csv'!E5</f>
+        <v>0.628</v>
+      </c>
+      <c r="T8" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y8,"0.000"),", ",TEXT(Z8,"0.000"),")")</f>
+        <v>(0.577, 0.685)</v>
+      </c>
+      <c r="U8" s="1">
+        <f>'tb_incidence_news_high - csv'!F5</f>
+        <v>2.7411049999999999E-2</v>
+      </c>
+      <c r="V8" s="1">
+        <f>'tb_incidence_news_high - csv'!G5</f>
+        <v>-10.648666</v>
+      </c>
+      <c r="W8" s="1">
+        <f>'tb_incidence_news_high - csv'!H5</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I5</f>
+        <v>***</v>
+      </c>
+      <c r="Y8" s="1">
+        <f>'tb_incidence_news_high - csv'!J5</f>
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="Z8" s="1">
+        <f>'tb_incidence_news_high - csv'!K5</f>
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B8" t="str">
+    <row r="9" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B6</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D9" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C6</f>
         <v>2.ccot_shift_pattern</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E9" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D6</f>
         <v>(firstnm) ccot_shift_pattern</v>
       </c>
-      <c r="F8">
+      <c r="F9" s="1">
         <f>'tb_incidence_news_all - csv'!E6</f>
         <v>0.69699999999999995</v>
       </c>
-      <c r="G8">
+      <c r="G9" s="1">
         <f>'tb_incidence_news_all - csv'!F6</f>
         <v>2.2093270000000002E-2</v>
       </c>
-      <c r="H8">
+      <c r="H9" s="1">
         <f>'tb_incidence_news_all - csv'!G6</f>
         <v>-11.390985000000001</v>
       </c>
-      <c r="I8">
+      <c r="I9" s="1">
         <f>'tb_incidence_news_all - csv'!H6</f>
         <v>0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J9" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I6</f>
         <v>***</v>
       </c>
-      <c r="K8">
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>(0.655, 0.742)</v>
+      </c>
+      <c r="L9" s="8">
         <f>'tb_incidence_news_all - csv'!J6</f>
         <v>0.65500000000000003</v>
       </c>
-      <c r="L8">
+      <c r="M9" s="8">
         <f>'tb_incidence_news_all - csv'!K6</f>
         <v>0.74199999999999999</v>
       </c>
-      <c r="M8">
+      <c r="N9" s="1">
         <f>'tb_incidence_news_all - csv'!L6</f>
         <v>1</v>
       </c>
-      <c r="N8">
+      <c r="O9" s="1">
         <f>'tb_incidence_news_all - csv'!M6</f>
         <v>1</v>
       </c>
-      <c r="O8">
+      <c r="P9" s="1">
         <f>'tb_incidence_news_all - csv'!N6</f>
         <v>0</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>14</v>
+      <c r="Q9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" s="1">
+        <f>'tb_incidence_news_high - csv'!E6</f>
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y9,"0.000"),", ",TEXT(Z9,"0.000"),")")</f>
+        <v>(0.672, 0.783)</v>
+      </c>
+      <c r="U9" s="1">
+        <f>'tb_incidence_news_high - csv'!F6</f>
+        <v>2.809385E-2</v>
+      </c>
+      <c r="V9" s="1">
+        <f>'tb_incidence_news_high - csv'!G6</f>
+        <v>-8.2867850000000001</v>
+      </c>
+      <c r="W9" s="1">
+        <f>'tb_incidence_news_high - csv'!H6</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I6</f>
+        <v>***</v>
+      </c>
+      <c r="Y9" s="1">
+        <f>'tb_incidence_news_high - csv'!J6</f>
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="Z9" s="1">
+        <f>'tb_incidence_news_high - csv'!K6</f>
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" t="str">
+    <row r="10" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B7</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D10" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C7</f>
         <v>3b.ccot_shift_pattern</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E10" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D7</f>
         <v>(firstnm) ccot_shift_pattern</v>
       </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9">
-        <f>'tb_incidence_news_all - csv'!F7</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>'tb_incidence_news_all - csv'!G7</f>
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <f>'tb_incidence_news_all - csv'!I7</f>
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <f>'tb_incidence_news_all - csv'!L7</f>
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <f>'tb_incidence_news_all - csv'!M7</f>
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <f>'tb_incidence_news_all - csv'!N7</f>
-        <v>0</v>
-      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="S10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AD10" s="3"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B10" t="str">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B8</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D11" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C8</f>
         <v>cmp_beds_max_c</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E11" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D8</f>
         <v>(p 50) cmp_beds_max_c</v>
       </c>
-      <c r="F10">
+      <c r="F11" s="1">
         <f>'tb_incidence_news_all - csv'!E8</f>
         <v>0.98799999999999999</v>
       </c>
-      <c r="G10">
+      <c r="G11" s="1">
         <f>'tb_incidence_news_all - csv'!F8</f>
         <v>2.1292799999999999E-3</v>
       </c>
-      <c r="H10">
+      <c r="H11" s="1">
         <f>'tb_incidence_news_all - csv'!G8</f>
         <v>-5.6957205999999996</v>
       </c>
-      <c r="I10">
+      <c r="I11" s="1">
         <f>'tb_incidence_news_all - csv'!H8</f>
         <v>0</v>
       </c>
-      <c r="J10" t="str">
+      <c r="J11" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I8</f>
         <v>***</v>
       </c>
-      <c r="K10">
+      <c r="K11" s="1" t="str">
+        <f t="shared" ref="K11:K14" si="1">CONCATENATE("(",TEXT(L11,"0.000"),", ",TEXT(M11,"0.000"),")")</f>
+        <v>(0.984, 0.992)</v>
+      </c>
+      <c r="L11" s="8">
         <f>'tb_incidence_news_all - csv'!J8</f>
         <v>0.98399999999999999</v>
       </c>
-      <c r="L10">
+      <c r="M11" s="8">
         <f>'tb_incidence_news_all - csv'!K8</f>
         <v>0.99199999999999999</v>
       </c>
-      <c r="M10">
+      <c r="N11" s="1">
         <f>'tb_incidence_news_all - csv'!L8</f>
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="O11" s="1">
         <f>'tb_incidence_news_all - csv'!M8</f>
         <v>1</v>
       </c>
-      <c r="O10">
+      <c r="P11" s="1">
         <f>'tb_incidence_news_all - csv'!N8</f>
         <v>0</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>14</v>
+      <c r="Q11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S11" s="1">
+        <f>'tb_incidence_news_high - csv'!E8</f>
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="T11" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y11,"0.000"),", ",TEXT(Z11,"0.000"),")")</f>
+        <v>(0.984, 0.994)</v>
+      </c>
+      <c r="U11" s="1">
+        <f>'tb_incidence_news_high - csv'!F8</f>
+        <v>2.56076E-3</v>
+      </c>
+      <c r="V11" s="1">
+        <f>'tb_incidence_news_high - csv'!G8</f>
+        <v>-4.1931203000000004</v>
+      </c>
+      <c r="W11" s="1">
+        <f>'tb_incidence_news_high - csv'!H8</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I8</f>
+        <v>***</v>
+      </c>
+      <c r="Y11" s="1">
+        <f>'tb_incidence_news_high - csv'!J8</f>
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="Z11" s="1">
+        <f>'tb_incidence_news_high - csv'!K8</f>
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" t="str">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B9</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D12" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C9</f>
         <v>winter</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E12" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D9</f>
         <v>Winter</v>
       </c>
-      <c r="F11">
+      <c r="F12" s="1">
         <f>'tb_incidence_news_all - csv'!E9</f>
         <v>1.091</v>
       </c>
-      <c r="G11">
+      <c r="G12" s="1">
         <f>'tb_incidence_news_all - csv'!F9</f>
         <v>3.1523460000000003E-2</v>
       </c>
-      <c r="H11">
+      <c r="H12" s="1">
         <f>'tb_incidence_news_all - csv'!G9</f>
         <v>3.0170313000000002</v>
       </c>
-      <c r="I11">
+      <c r="I12" s="1">
         <f>'tb_incidence_news_all - csv'!H9</f>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J11" t="str">
+      <c r="J12" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I9</f>
         <v>**</v>
       </c>
-      <c r="K11">
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(1.031, 1.155)</v>
+      </c>
+      <c r="L12" s="8">
         <f>'tb_incidence_news_all - csv'!J9</f>
         <v>1.0309999999999999</v>
       </c>
-      <c r="L11">
+      <c r="M12" s="8">
         <f>'tb_incidence_news_all - csv'!K9</f>
         <v>1.155</v>
       </c>
-      <c r="M11">
+      <c r="N12" s="1">
         <f>'tb_incidence_news_all - csv'!L9</f>
         <v>1</v>
       </c>
-      <c r="N11">
+      <c r="O12" s="1">
         <f>'tb_incidence_news_all - csv'!M9</f>
         <v>1</v>
       </c>
-      <c r="O11">
+      <c r="P12" s="1">
         <f>'tb_incidence_news_all - csv'!N9</f>
         <v>0</v>
       </c>
-      <c r="P11" s="1">
-        <f>I11</f>
+      <c r="Q12" s="3">
+        <f>I12</f>
         <v>3.0000000000000001E-3</v>
       </c>
+      <c r="S12" s="1">
+        <f>'tb_incidence_news_high - csv'!E9</f>
+        <v>1.1830000000000001</v>
+      </c>
+      <c r="T12" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y12,"0.000"),", ",TEXT(Z12,"0.000"),")")</f>
+        <v>(1.105, 1.266)</v>
+      </c>
+      <c r="U12" s="1">
+        <f>'tb_incidence_news_high - csv'!F9</f>
+        <v>4.1053439999999997E-2</v>
+      </c>
+      <c r="V12" s="1">
+        <f>'tb_incidence_news_high - csv'!G9</f>
+        <v>4.8401180999999998</v>
+      </c>
+      <c r="W12" s="1">
+        <f>'tb_incidence_news_high - csv'!H9</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I9</f>
+        <v>***</v>
+      </c>
+      <c r="Y12" s="1">
+        <f>'tb_incidence_news_high - csv'!J9</f>
+        <v>1.105</v>
+      </c>
+      <c r="Z12" s="1">
+        <f>'tb_incidence_news_high - csv'!K9</f>
+        <v>1.266</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" t="str">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B13" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B10</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="str">
+      <c r="D13" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!C10</f>
         <v>weekend</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E13" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!D10</f>
         <v>Day of week</v>
       </c>
-      <c r="F12">
+      <c r="F13" s="1">
         <f>'tb_incidence_news_all - csv'!E10</f>
         <v>0.83</v>
       </c>
-      <c r="G12">
+      <c r="G13" s="1">
         <f>'tb_incidence_news_all - csv'!F10</f>
         <v>1.528533E-2</v>
       </c>
-      <c r="H12">
+      <c r="H13" s="1">
         <f>'tb_incidence_news_all - csv'!G10</f>
         <v>-10.14268</v>
       </c>
-      <c r="I12">
+      <c r="I13" s="1">
         <f>'tb_incidence_news_all - csv'!H10</f>
         <v>0</v>
       </c>
-      <c r="J12" t="str">
+      <c r="J13" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!I10</f>
         <v>***</v>
       </c>
-      <c r="K12">
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>(0.800, 0.860)</v>
+      </c>
+      <c r="L13" s="8">
         <f>'tb_incidence_news_all - csv'!J10</f>
         <v>0.8</v>
       </c>
-      <c r="L12">
+      <c r="M13" s="8">
         <f>'tb_incidence_news_all - csv'!K10</f>
         <v>0.86</v>
       </c>
-      <c r="M12">
+      <c r="N13" s="1">
         <f>'tb_incidence_news_all - csv'!L10</f>
         <v>1</v>
       </c>
-      <c r="N12">
+      <c r="O13" s="1">
         <f>'tb_incidence_news_all - csv'!M10</f>
         <v>1</v>
       </c>
-      <c r="O12">
+      <c r="P13" s="1">
         <f>'tb_incidence_news_all - csv'!N10</f>
         <v>0</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>14</v>
+      <c r="Q13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="1">
+        <f>'tb_incidence_news_high - csv'!E10</f>
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="T13" s="1" t="str">
+        <f>CONCATENATE("(",TEXT(Y13,"0.000"),", ",TEXT(Z13,"0.000"),")")</f>
+        <v>(0.818, 0.918)</v>
+      </c>
+      <c r="U13" s="1">
+        <f>'tb_incidence_news_high - csv'!F10</f>
+        <v>2.540038E-2</v>
+      </c>
+      <c r="V13" s="1">
+        <f>'tb_incidence_news_high - csv'!G10</f>
+        <v>-4.8757447999999997</v>
+      </c>
+      <c r="W13" s="1">
+        <f>'tb_incidence_news_high - csv'!H10</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f>'tb_incidence_news_high - csv'!I10</f>
+        <v>***</v>
+      </c>
+      <c r="Y13" s="1">
+        <f>'tb_incidence_news_high - csv'!J10</f>
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="Z13" s="1">
+        <f>'tb_incidence_news_high - csv'!K10</f>
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B13" t="str">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="str">
         <f>'tb_incidence_news_all - csv'!B11</f>
         <v>NEWS risk all</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="str">
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!C11</f>
         <v>_cons</v>
       </c>
-      <c r="E13" t="str">
+      <c r="E14" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!D11</f>
         <v>Constant</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="4">
         <f>'tb_incidence_news_all - csv'!E11</f>
         <v>1.655</v>
       </c>
-      <c r="G13">
+      <c r="G14" s="4">
         <f>'tb_incidence_news_all - csv'!F11</f>
         <v>6.5434309999999996E-2</v>
       </c>
-      <c r="H13">
+      <c r="H14" s="4">
         <f>'tb_incidence_news_all - csv'!G11</f>
         <v>12.734897999999999</v>
       </c>
-      <c r="I13">
+      <c r="I14" s="4">
         <f>'tb_incidence_news_all - csv'!H11</f>
         <v>0</v>
       </c>
-      <c r="J13" t="str">
+      <c r="J14" s="4" t="str">
         <f>'tb_incidence_news_all - csv'!I11</f>
         <v>***</v>
       </c>
-      <c r="K13">
+      <c r="K14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>(1.531, 1.788)</v>
+      </c>
+      <c r="L14" s="11">
         <f>'tb_incidence_news_all - csv'!J11</f>
         <v>1.5309999999999999</v>
       </c>
-      <c r="L13">
+      <c r="M14" s="11">
         <f>'tb_incidence_news_all - csv'!K11</f>
         <v>1.788</v>
       </c>
-      <c r="M13">
+      <c r="N14" s="4">
         <f>'tb_incidence_news_all - csv'!L11</f>
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="O14" s="4">
         <f>'tb_incidence_news_all - csv'!M11</f>
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="P14" s="4">
         <f>'tb_incidence_news_all - csv'!N11</f>
         <v>0</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="4">
+        <f>'tb_incidence_news_high - csv'!E11</f>
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="T14" s="4" t="str">
+        <f>CONCATENATE("(",TEXT(Y14,"0.000"),", ",TEXT(Z14,"0.000"),")")</f>
+        <v>(0.523, 0.593)</v>
+      </c>
+      <c r="U14" s="4">
+        <f>'tb_incidence_news_high - csv'!F11</f>
+        <v>1.7731009999999998E-2</v>
+      </c>
+      <c r="V14" s="4">
+        <f>'tb_incidence_news_high - csv'!G11</f>
+        <v>-18.386959000000001</v>
+      </c>
+      <c r="W14" s="4">
+        <f>'tb_incidence_news_high - csv'!H11</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f>'tb_incidence_news_high - csv'!I11</f>
+        <v>***</v>
+      </c>
+      <c r="Y14" s="4">
+        <f>'tb_incidence_news_high - csv'!J11</f>
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="Z14" s="4">
+        <f>'tb_incidence_news_high - csv'!K11</f>
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.15">
+      <c r="AA15" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="S10:AA10"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="S2:AA2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2045,7 +2575,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>